<commit_message>
Initial attempt to plot character paths across 3 maps. Lots of issues.
</commit_message>
<xml_diff>
--- a/data/SceneDetail.xlsx
+++ b/data/SceneDetail.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\808Projects\OneOffs\JurassicPark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\808Projects\OneOffs\JurassicPark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE1FF5D-DD65-4235-8A22-C00AA9E54CA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1967,10 +1968,10 @@
   <dimension ref="A1:BE166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H13" sqref="H13"/>
+      <selection pane="bottomRight" activeCell="E103" sqref="E103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9230,7 +9231,9 @@
       <c r="D102" s="17">
         <v>34</v>
       </c>
-      <c r="E102" s="17"/>
+      <c r="E102" s="17">
+        <v>0</v>
+      </c>
       <c r="F102" s="14" t="s">
         <v>147</v>
       </c>

</xml_diff>

<commit_message>
Text cleanup for scenes and map
</commit_message>
<xml_diff>
--- a/data/SceneDetail.xlsx
+++ b/data/SceneDetail.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\808Projects\OneOffs\JurassicPark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFE1FF5D-DD65-4235-8A22-C00AA9E54CA5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7F183-18E9-4B08-BD92-1EAFF06085DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SceneDetail" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="333">
   <si>
     <t>1EXTJUNGLENIGHT</t>
   </si>
@@ -1013,9 +1013,6 @@
   </si>
   <si>
     <t>CREDITS</t>
-  </si>
-  <si>
-    <t>Café</t>
   </si>
   <si>
     <t>Brachiosaurus hill</t>
@@ -1968,10 +1965,10 @@
   <dimension ref="A1:BE166"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E103" sqref="E103"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2665,8 +2662,9 @@
       <c r="G8" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>331</v>
+      <c r="H8" s="14" t="str">
+        <f>"Cafe"</f>
+        <v>Cafe</v>
       </c>
       <c r="I8" s="14" t="s">
         <v>200</v>
@@ -2953,7 +2951,7 @@
         <v>151</v>
       </c>
       <c r="H12" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>201</v>
@@ -5420,7 +5418,7 @@
         <v>151</v>
       </c>
       <c r="H46" s="14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="I46" s="14" t="s">
         <v>202</v>
@@ -8622,7 +8620,7 @@
         <v>151</v>
       </c>
       <c r="H92" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I92" s="14" t="s">
         <v>207</v>
@@ -8688,7 +8686,7 @@
         <v>151</v>
       </c>
       <c r="H93" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I93" s="14" t="s">
         <v>207</v>
@@ -8927,7 +8925,7 @@
         <v>151</v>
       </c>
       <c r="H97" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I97" s="14" t="s">
         <v>239</v>
@@ -9046,7 +9044,7 @@
         <v>151</v>
       </c>
       <c r="H99" s="14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="I99" s="14" t="s">
         <v>239</v>

</xml_diff>

<commit_message>
Changed location name of helicopter
</commit_message>
<xml_diff>
--- a/data/SceneDetail.xlsx
+++ b/data/SceneDetail.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Documents\808Projects\OneOffs\JurassicPark\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DD7F183-18E9-4B08-BD92-1EAFF06085DF}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1DC9C4-B704-4CFF-9607-71CD954D8E28}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10050" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SceneDetail" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">SceneDetail!$A$1:$BE$165</definedName>
+  </definedNames>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
@@ -1968,7 +1971,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomRight" activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12711,7 +12714,7 @@
         <v>151</v>
       </c>
       <c r="H165" s="14" t="s">
-        <v>260</v>
+        <v>169</v>
       </c>
       <c r="I165" s="1" t="s">
         <v>256</v>

</xml_diff>